<commit_message>
Add functions to set and get the randomized indices for the CompositeIndicesList; Update documentation; Ready for switch from _l2iPageQuestionCompositeIndices to _l3iPageQuestionGroupCompositeIndices
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5373691A-4E5D-4770-9C8C-4DAE060AEB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A9B32-2128-403B-AC66-E325EE973117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3312" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44589</v>
+        <v>44592</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Remove tracking of Shutdown batch file; Update to Elements and Attributes
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031A9B32-2128-403B-AC66-E325EE973117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895BB795-A5CD-42DF-90A7-D27BEAB9B7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -263,9 +263,6 @@
     <t>PageGroup</t>
   </si>
   <si>
-    <t>For randomizing pages if some pages need to remain together. PageGroup numbers of 0 will not be randomized and will be the first in the sequence of pages</t>
-  </si>
-  <si>
     <t>LoginTime</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
   </si>
   <si>
     <t>all other formats are read in as a 'Data' volume (NRRD, NIFTI, MHD...) ; Even a dicom slice can be read in as a Data volume by setting this to 'N' and setting the attribute 'Type' to 'Volume'</t>
-  </si>
-  <si>
-    <t>(integer value 0 included)</t>
   </si>
   <si>
     <r>
@@ -308,9 +302,6 @@
     <t>Foreground, Background, Label, Segmentation (default=Background)</t>
   </si>
   <si>
-    <t>If "Y", PageGroup attribute must exist in Page element; Pages (other than 0) will be randomized; If element RandomizedPageGroupIndices exists under Session element, those indices will be used to order the pages.</t>
-  </si>
-  <si>
     <t>these paths are relative to the parent directory selected by the user when logging in; if DicomRead="Y", path to one slice of the DICOM series is defined here</t>
   </si>
   <si>
@@ -369,6 +360,15 @@
   </si>
   <si>
     <t>logout timestamp reflecting the last time a save was done to the user's response xml</t>
+  </si>
+  <si>
+    <t>If "Y", PageGroup attribute must exist in Page element; Pages (other than 0) will be randomized; If element RandomizedPageGroupIndices exists under Session element, those indices will be used to order the pages. All elements set to PageGroup=0 will be filtered to the beginning of the quiz - in the order they are assigned in the quiz.</t>
+  </si>
+  <si>
+    <t>(integer value, 0 included)</t>
+  </si>
+  <si>
+    <t>For randomizing pages if some pages need to remain together (example: Patient1 - Planning CT followed by Patient1 - Follow-up CT). PageGroup numbers of 0 will not be randomized and will be the first in the sequence of pages</t>
   </si>
 </sst>
 </file>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +869,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44592</v>
+        <v>44601</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,7 +901,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>44</v>
@@ -926,7 +926,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -940,7 +940,7 @@
         <v>31</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -995,7 +995,7 @@
         <v>31</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1024,10 +1024,10 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1065,7 +1065,7 @@
         <v>31</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1148,7 +1148,7 @@
         <v>61</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1192,7 +1192,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I23" s="12"/>
     </row>
@@ -1212,7 +1212,7 @@
         <v>22</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1233,7 +1233,7 @@
         <v>30</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1250,7 +1250,7 @@
         <v>21</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1269,7 +1269,7 @@
         <v>16</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1286,7 +1286,7 @@
         <v>16</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
         <v>31</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -1313,14 +1313,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
         <v>32</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1339,7 +1339,7 @@
         <v>16</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1430,33 +1430,33 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I39" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1464,10 +1464,10 @@
         <v>0</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F42" s="18" t="s">
         <v>1</v>
@@ -1483,7 +1483,7 @@
         <v>52</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -1491,7 +1491,7 @@
         <v>53</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -1499,7 +1499,7 @@
         <v>54</v>
       </c>
       <c r="F46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -1510,23 +1510,23 @@
         <v>20</v>
       </c>
       <c r="E48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.3">
@@ -1534,10 +1534,10 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H52" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.3">
@@ -1545,18 +1545,18 @@
         <v>54</v>
       </c>
       <c r="F53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F54" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify required location of a custom ROIColorFile to be in the same directory as the customized Quiz being opened. ; This allows the study coordinator to keep customized quiz and color file together. ; (Previously, the coordinator would have to load a customized color tabl into the Image Quizzer Resources/ColorFiles folder.)
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895BB795-A5CD-42DF-90A7-D27BEAB9B7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F5F2C-1F7B-4476-B542-A1D458DF87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
   <si>
     <t>Element</t>
   </si>
@@ -169,12 +169,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>eg. Pi-RadsStudy.txt, LungSABRStudy.txt, GenericColors.txt (default)</t>
-  </si>
-  <si>
-    <t>syntax: number descriptor r g b a</t>
   </si>
   <si>
     <t xml:space="preserve">… </t>
@@ -296,9 +290,6 @@
     </r>
   </si>
   <si>
-    <t>view Slicer MRML nodes in the Data module to get Slicer's list; these are case sensitive</t>
-  </si>
-  <si>
     <t>Foreground, Background, Label, Segmentation (default=Background)</t>
   </si>
   <si>
@@ -369,6 +360,44 @@
   </si>
   <si>
     <t>For randomizing pages if some pages need to remain together (example: Patient1 - Planning CT followed by Patient1 - Follow-up CT). PageGroup numbers of 0 will not be randomized and will be the first in the sequence of pages</t>
+  </si>
+  <si>
+    <t>Opacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal value between 0 and 1.0; This only is effective on images assigned to Layer=Foreground </t>
+  </si>
+  <si>
+    <t>Defining the ColorTable modifies how the image is displayed in the viewing window; view Slicer MRML nodes in the Data module to get Slicer's list of available color maps; these are case sensitive</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">string holding name of the color file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>without</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the .txt extension (eg. "Pi-RadsStudy" for the Pi-RadsStudy.txt color file; if empty or doesn't exist, the Image Quizzer's Generic colors table will be used)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> file must be located in the same directory as the assigned quiz directory (eg. C:\pathToQuiz\newColorFIle.txt);   example syntax for each color (one line per color: number descriptor r g b a): 3 PI-RADS_intermediate 177 122 101 255 </t>
   </si>
 </sst>
 </file>
@@ -841,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +898,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44601</v>
+        <v>44619</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,13 +930,13 @@
         <v>33</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -920,10 +949,10 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -933,14 +962,14 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -961,7 +990,7 @@
         <v>43</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -975,10 +1004,10 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -995,7 +1024,7 @@
         <v>31</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1005,11 +1034,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -1020,14 +1049,14 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1045,10 +1074,10 @@
         <v>34</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1058,14 +1087,14 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="12" t="s">
         <v>31</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1092,14 +1121,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1109,14 +1138,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1134,7 +1163,7 @@
       </c>
       <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1145,39 +1174,39 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I22" s="12"/>
     </row>
@@ -1186,178 +1215,176 @@
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>77</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="14" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H26" s="12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>94</v>
+        <v>28</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="12" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G32" s="2"/>
       <c r="H32" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
@@ -1366,11 +1393,13 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="H33" s="12" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I33" s="12"/>
     </row>
@@ -1381,7 +1410,7 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
@@ -1394,28 +1423,32 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="1"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="12"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
+      <c r="I36" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="15"/>
@@ -1428,135 +1461,146 @@
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+      <c r="G40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" t="s">
-        <v>90</v>
-      </c>
-      <c r="F39" t="s">
-        <v>90</v>
-      </c>
-      <c r="G39" t="s">
-        <v>90</v>
-      </c>
-      <c r="H39" t="s">
-        <v>90</v>
-      </c>
-      <c r="I39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E42" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="18" t="s">
+      <c r="F43" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C43" t="s">
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
         <v>4</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
+        <v>50</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
         <v>52</v>
       </c>
-      <c r="H43" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D44" t="s">
-        <v>53</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
+      <c r="F47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>18</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>20</v>
       </c>
-      <c r="E48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F49" t="s">
-        <v>85</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>87</v>
+      <c r="E49" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F50" t="s">
+        <v>82</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>66</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
         <v>68</v>
       </c>
-      <c r="H50" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s">
-        <v>70</v>
-      </c>
-      <c r="H52" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D53" t="s">
-        <v>54</v>
-      </c>
-      <c r="F53" t="s">
-        <v>68</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>86</v>
+      <c r="H53" s="17" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D54" t="s">
+        <v>52</v>
+      </c>
       <c r="F54" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>92</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified attributes : AllowMultipleResponse now defaults to "N"; SegmentRequired had the name changed to EnableSegmentEditor; Test XML's were updated to reflect these changes; Fixed in Session>GetQuestionSetResponseCompletionLevel the clearing of _lsPreviousResponses ; This has to be cleared at the start of each new question set in order for the quiz to resume in the proper location if the user exited the quiz prematurely.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638F5F2C-1F7B-4476-B542-A1D458DF87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AFBAB5-D3EE-4DA1-9A55-807FC3F27CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
   <si>
     <t>Element</t>
   </si>
@@ -120,9 +120,6 @@
     <t>RotateToAcquisition</t>
   </si>
   <si>
-    <t>SegmentRequired</t>
-  </si>
-  <si>
     <t>ColorTable</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
   </si>
   <si>
     <t>Y,N (default=N)</t>
-  </si>
-  <si>
-    <t>Y,N (default=Y)</t>
   </si>
   <si>
     <t>Required</t>
@@ -308,9 +302,6 @@
     <t>If "Y", the SegmentEditor tab becomes enabled in the quiz</t>
   </si>
   <si>
-    <t>If "Y", the quiz allows the user to press Previous button and responses on that page are allowed to be edited. If "N", pressing Previous will display the previous responses but will not allow the user to edit them</t>
-  </si>
-  <si>
     <t>string is displayed in the question box</t>
   </si>
   <si>
@@ -398,6 +389,18 @@
   </si>
   <si>
     <t xml:space="preserve"> file must be located in the same directory as the assigned quiz directory (eg. C:\pathToQuiz\newColorFIle.txt);   example syntax for each color (one line per color: number descriptor r g b a): 3 PI-RADS_intermediate 177 122 101 255 </t>
+  </si>
+  <si>
+    <t>EnableSegmentEditor</t>
+  </si>
+  <si>
+    <t>If "Y", the quiz allows the user to press Previous button and responses on that page are allowed to be edited. If "N" (default), pressing Previous will display the previous responses but will not allow the user to edit them</t>
+  </si>
+  <si>
+    <t>SegmentRequired</t>
+  </si>
+  <si>
+    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it)</t>
   </si>
 </sst>
 </file>
@@ -870,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,19 +894,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44619</v>
+        <v>44643</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -927,13 +930,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
@@ -945,14 +948,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -962,14 +965,14 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -981,16 +984,16 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1004,10 +1007,10 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1021,10 +1024,10 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1034,11 +1037,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -1049,14 +1052,14 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1068,16 +1071,16 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1087,14 +1090,14 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1107,7 +1110,7 @@
         <v>26</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>17</v>
@@ -1121,14 +1124,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1138,14 +1141,14 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1159,7 +1162,7 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" s="12"/>
     </row>
@@ -1170,14 +1173,14 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -1187,12 +1190,12 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1206,7 +1209,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I22" s="12"/>
     </row>
@@ -1221,7 +1224,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I23" s="12"/>
     </row>
@@ -1236,7 +1239,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="2"/>
       <c r="H24" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I24" s="12"/>
     </row>
@@ -1250,13 +1253,13 @@
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
       <c r="G25" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>22</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1271,13 +1274,13 @@
         <v>23</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1294,7 +1297,7 @@
         <v>21</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1306,14 +1309,14 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1330,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1340,68 +1343,68 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="1" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>25</v>
+        <v>88</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="12" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G33" s="2"/>
       <c r="H33" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
@@ -1410,11 +1413,13 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G34" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H34" s="12" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I34" s="12"/>
     </row>
@@ -1425,11 +1430,11 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I35" s="12"/>
     </row>
@@ -1438,28 +1443,32 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="1"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="12"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
+      <c r="I37" s="12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="15"/>
@@ -1472,135 +1481,146 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" t="s">
+        <v>84</v>
+      </c>
+      <c r="H41" t="s">
+        <v>84</v>
+      </c>
+      <c r="I41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C44" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C40" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" t="s">
-        <v>87</v>
-      </c>
-      <c r="G40" t="s">
-        <v>87</v>
-      </c>
-      <c r="H40" t="s">
-        <v>87</v>
-      </c>
-      <c r="I40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="F43" s="18" t="s">
+      <c r="F44" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C44" t="s">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
         <v>50</v>
       </c>
-      <c r="H44" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D45" t="s">
-        <v>51</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>52</v>
-      </c>
-      <c r="F47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
+      <c r="F48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
         <v>18</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>20</v>
       </c>
-      <c r="E49" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F50" t="s">
-        <v>82</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>84</v>
+      <c r="E50" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F51" t="s">
+        <v>79</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>64</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" t="s">
         <v>66</v>
       </c>
-      <c r="H51" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>68</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D54" t="s">
-        <v>52</v>
-      </c>
-      <c r="F54" t="s">
-        <v>66</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>83</v>
+      <c r="H54" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
       <c r="F55" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>93</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>89</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added setup for SegmentRequired attribute in the Image element. Validation code added.; Updated documentation in excel spreadsheet and the xml schema file
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5AFBAB5-D3EE-4DA1-9A55-807FC3F27CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB432AB6-60DA-4CE7-8A62-95399D6ECA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="107">
   <si>
     <t>Element</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>searches history for an image with a LabelMapID attribute that matches this string</t>
-  </si>
-  <si>
-    <t>ID string used for matching if subsequent Image needs this Label Map displayed</t>
   </si>
   <si>
     <t>State</t>
@@ -299,9 +296,6 @@
     <t>string is displayed in the question set box</t>
   </si>
   <si>
-    <t>If "Y", the SegmentEditor tab becomes enabled in the quiz</t>
-  </si>
-  <si>
     <t>string is displayed in the question box</t>
   </si>
   <si>
@@ -394,13 +388,31 @@
     <t>EnableSegmentEditor</t>
   </si>
   <si>
-    <t>If "Y", the quiz allows the user to press Previous button and responses on that page are allowed to be edited. If "N" (default), pressing Previous will display the previous responses but will not allow the user to edit them</t>
-  </si>
-  <si>
     <t>SegmentRequired</t>
   </si>
   <si>
-    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it)</t>
+    <t>If "Y", the SegmentEditor tab becomes enabled in the quiz; This applies to all question sets on the page</t>
+  </si>
+  <si>
+    <t>If "Y", the quiz allows the user to press Previous button and responses on that page are allowed to be edited. If "N" (default), pressing Previous will display the previous responses but will not allow the user to edit them; This applies to all question sets on that page.</t>
+  </si>
+  <si>
+    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required</t>
+  </si>
+  <si>
+    <t>QuizComplete</t>
+  </si>
+  <si>
+    <t>PageComplete</t>
+  </si>
+  <si>
+    <t>all questions have been answered and required segments have been created</t>
+  </si>
+  <si>
+    <t>All pages have completed questions and segments (where required)</t>
+  </si>
+  <si>
+    <t>ID string used for matching if subsequent Image needs this Label Map displayed; (If more than one image element is set up for this image path - differing orientations, this attribute only needs to be set up on one instance)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -557,6 +569,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -873,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +917,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44643</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -933,7 +949,7 @@
         <v>31</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>42</v>
@@ -952,10 +968,10 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
@@ -965,14 +981,14 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -993,7 +1009,7 @@
         <v>41</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1010,7 +1026,7 @@
         <v>43</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1027,7 +1043,7 @@
         <v>30</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1037,11 +1053,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -1052,288 +1068,286 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G14" s="2"/>
       <c r="H14" s="12" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" s="13"/>
+        <v>97</v>
+      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="12" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H18" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G19" s="13"/>
       <c r="H19" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="12" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="12"/>
+      <c r="I23" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="I25" s="12"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="2"/>
       <c r="H26" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="I26" s="12"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="I27" s="12"/>
+    </row>
+    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G28" s="2"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="H28" s="12" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="I28" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H29" s="12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1341,50 +1355,52 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="E30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="1" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="12" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="12" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -1403,7 +1419,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -1467,7 +1483,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1494,33 +1510,33 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B42" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
@@ -1528,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F44" s="18" t="s">
         <v>1</v>
@@ -1539,88 +1555,118 @@
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" t="s">
-        <v>48</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>49</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>78</v>
-      </c>
+    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+    </row>
+    <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="19"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>50</v>
-      </c>
-      <c r="F48" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D49" t="s">
+        <v>48</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>49</v>
+      </c>
       <c r="F51" t="s">
-        <v>79</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="52" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F52" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
         <v>2</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D58" t="s">
+        <v>65</v>
+      </c>
+      <c r="H58" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="H54" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D55" t="s">
-        <v>50</v>
-      </c>
-      <c r="F55" t="s">
-        <v>64</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F56" t="s">
-        <v>89</v>
-      </c>
-      <c r="H56" s="10" t="s">
-        <v>90</v>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>87</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP  - Rough work done in PageState to test the completion level of LabelMap segmentation
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB432AB6-60DA-4CE7-8A62-95399D6ECA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE776EE0-0AFE-4CFA-9613-4F8651058C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="1680" windowWidth="17280" windowHeight="9972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
   <si>
     <t>Element</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>ID string used for matching if subsequent Image needs this Label Map displayed; (If more than one image element is set up for this image path - differing orientations, this attribute only needs to be set up on one instance)</t>
+  </si>
+  <si>
+    <t>SegmentRequiredOnAnyImage</t>
+  </si>
+  <si>
+    <t>If "Y", there must be one non-empty labelmap file created for any of the images on the page. If a labelmap file was redisplayed from a previous page (and it is the only label map file for that page), it must be modified.</t>
   </si>
 </sst>
 </file>
@@ -889,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -902,7 +908,7 @@
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.21875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="73.88671875" style="10" customWidth="1"/>
     <col min="9" max="9" width="40" style="10" customWidth="1"/>
@@ -917,7 +923,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44663</v>
+        <v>44664</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1112,186 +1118,188 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="12" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H17" s="12" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G18" s="13"/>
       <c r="H18" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H19" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G20" s="13"/>
       <c r="H20" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="G23" s="2"/>
-      <c r="H23" s="12"/>
+      <c r="H23" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="I23" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="H24" s="12"/>
       <c r="I24" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="12"/>
+        <v>30</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="1"/>
       <c r="G26" s="2"/>
       <c r="H26" s="12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I26" s="12"/>
     </row>
@@ -1300,100 +1308,98 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="1"/>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="I27" s="12"/>
     </row>
-    <row r="28" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>71</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="6" t="s">
+      <c r="F29" s="1"/>
+      <c r="G29" s="14" t="s">
         <v>32</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="2"/>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H30" s="12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="2"/>
       <c r="H31" s="12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="12" t="s">
@@ -1407,9 +1413,7 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="1" t="s">
         <v>25</v>
@@ -1419,25 +1423,27 @@
         <v>16</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
@@ -1446,11 +1452,13 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G35" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H35" s="12" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="I35" s="12"/>
     </row>
@@ -1461,7 +1469,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="12" t="s">
@@ -1474,28 +1482,32 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="1"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="12" t="s">
+      <c r="I38" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="15"/>
@@ -1508,164 +1520,175 @@
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>82</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>82</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>82</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>82</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>82</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G42" t="s">
         <v>82</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>82</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I42" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="18" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="18" t="s">
+    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D45" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="18" t="s">
+      <c r="E45" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F45" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-    </row>
-    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H45" s="19"/>
       <c r="I45" s="19"/>
     </row>
     <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="20" t="s">
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+    </row>
+    <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F47" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="I46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="H47" s="21"/>
       <c r="I47" s="19"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
+    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>4</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>47</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H49" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D49" t="s">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D50" t="s">
         <v>48</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H50" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
         <v>49</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F52" t="s">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
         <v>102</v>
       </c>
-      <c r="H52" s="10" t="s">
+      <c r="H53" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
         <v>18</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>20</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F55" t="s">
-        <v>77</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="56" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
+        <v>77</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
         <v>63</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H57" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
         <v>2</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="H58" s="17" t="s">
+      <c r="H59" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D59" t="s">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D60" t="s">
         <v>49</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>63</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="H60" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F60" t="s">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
         <v>87</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H61" s="10" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add GroupBox layout options (Horizontal or Vertical) for Radio or CheckBox type questions. All others default to the vertical layout.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE776EE0-0AFE-4CFA-9613-4F8651058C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1130542A-A81D-438D-9BD0-0C83FE41D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1680" windowWidth="17280" windowHeight="9972" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
   <si>
     <t>Element</t>
   </si>
@@ -419,6 +419,15 @@
   </si>
   <si>
     <t>If "Y", there must be one non-empty labelmap file created for any of the images on the page. If a labelmap file was redisplayed from a previous page (and it is the only label map file for that page), it must be modified.</t>
+  </si>
+  <si>
+    <t>GroupLayout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for Question Type="Radio" or Type="CheckBox"; will display the options horizontally or vertically </t>
+  </si>
+  <si>
+    <t>Horizontal, Vertical (default=Vertical)</t>
   </si>
 </sst>
 </file>
@@ -542,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -581,6 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -910,8 +920,8 @@
     <col min="5" max="5" width="11.77734375" customWidth="1"/>
     <col min="6" max="6" width="26.21875" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="73.88671875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="40" style="10" customWidth="1"/>
+    <col min="8" max="8" width="67" style="10" customWidth="1"/>
+    <col min="9" max="9" width="46" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -923,7 +933,7 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44664</v>
+        <v>44707</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1462,7 +1472,7 @@
       </c>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1472,12 +1482,12 @@
         <v>33</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="12" t="s">
+      <c r="H36" s="2"/>
+      <c r="I36" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="12"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1487,38 +1497,44 @@
         <v>34</v>
       </c>
       <c r="G37" s="2"/>
-      <c r="H37" s="12" t="s">
+      <c r="H37" s="2"/>
+      <c r="I37" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="12"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2" t="s">
+      <c r="E38" s="2"/>
+      <c r="F38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="12" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="12" t="s">
+      <c r="I39" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="15"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
@@ -1531,164 +1547,175 @@
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>82</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>82</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>82</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E43" t="s">
         <v>82</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F43" t="s">
         <v>82</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>82</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H43" t="s">
         <v>82</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="18" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B44" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="18" t="s">
+    <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D46" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="18" t="s">
+      <c r="E46" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F46" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-    </row>
-    <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="20" t="s">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F48" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="I47" s="19"/>
-    </row>
-    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="H48" s="21"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
+    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
         <v>4</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="10" t="s">
+      <c r="H50" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D50" t="s">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D51" t="s">
         <v>48</v>
       </c>
-      <c r="H50" s="10" t="s">
+      <c r="H51" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
         <v>49</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F53" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F53" t="s">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
         <v>102</v>
       </c>
-      <c r="H53" s="10" t="s">
+      <c r="H54" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
         <v>18</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>20</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E56" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F56" t="s">
+    <row r="57" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
         <v>77</v>
       </c>
-      <c r="H56" s="10" t="s">
+      <c r="H57" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F57" t="s">
+    <row r="58" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
         <v>63</v>
       </c>
-      <c r="H57" s="10" t="s">
+      <c r="H58" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
         <v>2</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>65</v>
       </c>
-      <c r="H59" s="17" t="s">
+      <c r="H60" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D60" t="s">
+    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D61" t="s">
         <v>49</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F61" t="s">
         <v>63</v>
       </c>
-      <c r="H60" s="10" t="s">
+      <c r="H61" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F61" t="s">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
         <v>87</v>
       </c>
-      <c r="H61" s="10" t="s">
+      <c r="H62" s="10" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP - AGAIN; Changes to separate how I keep track of the number of markup lines completed in l2iCompletedMarkupLines vs how I use this variable for the PageCompletion function. I'm using the same variable for two different things. I just added Validation for the markup lines attributes and updated the xml schema and excel documentation to reflect the coming changes. Stay tuned...
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1130542A-A81D-438D-9BD0-0C83FE41D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="117">
   <si>
     <t>Element</t>
   </si>
@@ -397,9 +396,6 @@
     <t>If "Y", the quiz allows the user to press Previous button and responses on that page are allowed to be edited. If "N" (default), pressing Previous will display the previous responses but will not allow the user to edit them; This applies to all question sets on that page.</t>
   </si>
   <si>
-    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required</t>
-  </si>
-  <si>
     <t>QuizComplete</t>
   </si>
   <si>
@@ -428,12 +424,30 @@
   </si>
   <si>
     <t>Horizontal, Vertical (default=Vertical)</t>
+  </si>
+  <si>
+    <t>The user must create a minimum number of lines. These can be created on any of the displayed images.</t>
+  </si>
+  <si>
+    <t>MinMarkupLinesRequired</t>
+  </si>
+  <si>
+    <t>MinMarkupLinesRequiredOnAnyImage</t>
+  </si>
+  <si>
+    <t>integer number (minimum = 1)</t>
+  </si>
+  <si>
+    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each</t>
+  </si>
+  <si>
+    <t>The user must create a minimum number of lines on the image specified. ; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -904,27 +918,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="G23" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="67" style="10" customWidth="1"/>
     <col min="9" max="9" width="46" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
@@ -933,16 +947,16 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44707</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44715</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:9" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -971,7 +985,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -990,7 +1004,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1007,7 +1021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1028,7 +1042,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1045,7 +1059,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1062,7 +1076,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1077,7 +1091,7 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1094,7 +1108,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1111,7 +1125,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1128,594 +1142,628 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="12" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="13"/>
+        <v>40</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H18" s="12" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="G19" s="13"/>
       <c r="H19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="13"/>
+        <v>26</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H20" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="G21" s="13"/>
       <c r="H21" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I23" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="1" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="I24" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G25" s="2"/>
-      <c r="H25" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I26" s="12"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="12"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="14" t="s">
-        <v>32</v>
-      </c>
+      <c r="G29" s="2"/>
       <c r="H29" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="I29" s="12"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="I30" s="12"/>
+    </row>
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="D31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="H31" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="H32" s="12" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="E33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="2"/>
       <c r="H33" s="12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="C34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
         <v>16</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G35" s="2"/>
       <c r="H35" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="12"/>
-    </row>
-    <row r="36" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="I35" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="12" t="s">
+        <v>16</v>
+      </c>
       <c r="I36" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="12"/>
+    </row>
+    <row r="38" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="1" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="G38" s="2"/>
-      <c r="H38" s="22" t="s">
-        <v>111</v>
-      </c>
+      <c r="H38" s="2"/>
       <c r="I38" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="2"/>
+      <c r="F39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="12" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="12" t="s">
+      <c r="I41" s="12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="15"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>82</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>82</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>82</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E45" t="s">
         <v>82</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F45" t="s">
         <v>82</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G45" t="s">
         <v>82</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H45" t="s">
         <v>82</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I45" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="18" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="18" t="s">
+    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C48" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D48" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E48" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F48" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-    </row>
-    <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-    </row>
-    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="20" t="s">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+    </row>
+    <row r="50" spans="3:9" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C50" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F50" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="H50" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>47</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>49</v>
+      </c>
+      <c r="F55" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+      <c r="H56" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="I48" s="19"/>
-    </row>
-    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="19"/>
-    </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>4</v>
-      </c>
-      <c r="D50" t="s">
-        <v>47</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D51" t="s">
-        <v>48</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>77</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>65</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>49</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D56" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F57" t="s">
-        <v>77</v>
-      </c>
-      <c r="H57" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F58" t="s">
-        <v>63</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>65</v>
-      </c>
-      <c r="H60" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="61" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="D61" t="s">
-        <v>49</v>
-      </c>
-      <c r="F61" t="s">
-        <v>63</v>
-      </c>
-      <c r="H61" s="10" t="s">
+      <c r="H63" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="F62" t="s">
+    <row r="64" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
         <v>87</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H64" s="10" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP - changed the completion list for markup lines to hold 3 element lists (instead of 2 like the segmentation completion list). - Changed the order of the completion lists s.t. the elements for segmentation are [ completedTF, requiredTF] and for the markup lines these are [completedTF, minimum required # of lines, current # of lines]. I wanted some kind of consistency between segmentation and markup lines completion lists. - Removed 'not applicable' code of -1 for images on the Segmentation or Label layer. These are now just set to 0 (not required)
More testing and cleanup required.....
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0486AF37-B718-45E6-B6FC-51D65D85DD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -438,16 +440,16 @@
     <t>integer number (minimum = 1)</t>
   </si>
   <si>
-    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each</t>
-  </si>
-  <si>
-    <t>The user must create a minimum number of lines on the image specified. ; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each</t>
+    <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each; This attribute is not applicable for images assigned to a Segmentation or Label layer;</t>
+  </si>
+  <si>
+    <t>The user must create a minimum number of lines on the image specified. ; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each; This attribute is not applicable for images assigned to a Segmentation or Label layer;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -918,27 +920,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G23" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="67" style="10" customWidth="1"/>
     <col min="9" max="9" width="46" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>37</v>
       </c>
@@ -947,16 +949,16 @@
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44715</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44718</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -985,7 +987,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1021,7 +1023,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1042,7 +1044,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1059,7 +1061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1076,7 +1078,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1091,7 +1093,7 @@
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1108,7 +1110,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1125,7 +1127,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1142,7 +1144,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1159,7 +1161,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1176,7 +1178,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -1197,7 +1199,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1214,7 +1216,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1231,7 +1233,7 @@
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1248,7 +1250,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1265,7 +1267,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1280,7 +1282,7 @@
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1297,7 +1299,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1312,7 +1314,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1329,7 +1331,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1346,7 +1348,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1361,7 +1363,7 @@
       </c>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1376,7 +1378,7 @@
       </c>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1391,7 +1393,7 @@
       </c>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1410,7 +1412,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1431,7 +1433,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1448,7 +1450,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
@@ -1467,7 +1469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1484,7 +1486,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1503,7 +1505,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1520,7 +1522,7 @@
       </c>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1535,7 +1537,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1550,7 +1552,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1567,7 +1569,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1584,7 +1586,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -1595,7 +1597,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -1606,7 +1608,7 @@
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>82</v>
       </c>
@@ -1632,12 +1634,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="18" t="s">
         <v>0</v>
       </c>
@@ -1653,11 +1655,11 @@
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="3:9" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="20" t="s">
         <v>3</v>
       </c>
@@ -1669,13 +1671,13 @@
       </c>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="20"/>
       <c r="F51" s="20"/>
       <c r="H51" s="21"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>4</v>
       </c>
@@ -1686,7 +1688,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>48</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
         <v>49</v>
       </c>
@@ -1702,7 +1704,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
       <c r="F56" t="s">
         <v>101</v>
       </c>
@@ -1710,7 +1712,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
         <v>18</v>
       </c>
@@ -1721,7 +1723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F59" t="s">
         <v>77</v>
       </c>
@@ -1729,7 +1731,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F60" t="s">
         <v>63</v>
       </c>
@@ -1737,7 +1739,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D63" t="s">
         <v>49</v>
       </c>
@@ -1759,7 +1761,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F64" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Changed XML element name from Destination and Orientation to DefaultDestination and DefaultOrientation; More XML's to be modified and tested
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0486AF37-B718-45E6-B6FC-51D65D85DD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,12 +49,6 @@
   </si>
   <si>
     <t>Image</t>
-  </si>
-  <si>
-    <t>Destination</t>
-  </si>
-  <si>
-    <t>Orientation</t>
   </si>
   <si>
     <t>Layer</t>
@@ -445,11 +438,17 @@
   <si>
     <t>The user must create a minimum number of lines on the image specified. ; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each; This attribute is not applicable for images assigned to a Segmentation or Label layer;</t>
   </si>
+  <si>
+    <t>DefaultDestination</t>
+  </si>
+  <si>
+    <t>DefaultOrientation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -920,74 +919,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="67" style="10" customWidth="1"/>
     <col min="9" max="9" width="46" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44718</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44749</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -996,34 +995,34 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>3</v>
@@ -1032,153 +1031,153 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -1187,406 +1186,406 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I28" s="12"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
       <c r="H29" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I29" s="12"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I30" s="12"/>
     </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
       <c r="G31" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="2"/>
       <c r="H33" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I37" s="12"/>
     </row>
-    <row r="38" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
       <c r="H41" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -1597,7 +1596,7 @@
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -1608,46 +1607,46 @@
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>1</v>
@@ -1655,118 +1654,118 @@
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H49" s="19"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:9" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="C50" s="20" t="s">
         <v>3</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="20"/>
       <c r="F51" s="20"/>
       <c r="H51" s="21"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>4</v>
       </c>
       <c r="D52" t="s">
+        <v>45</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>47</v>
       </c>
-      <c r="H52" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D53" t="s">
-        <v>48</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>49</v>
-      </c>
       <c r="F55" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="D58" t="s">
-        <v>20</v>
-      </c>
       <c r="E58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="59" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="H59" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="3:9" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="3:9" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="3:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating documentation; Some code cleanup
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -93,9 +93,6 @@
     <t>Option</t>
   </si>
   <si>
-    <t>(ROI name in RTStruct)</t>
-  </si>
-  <si>
     <t>(relative path to image data file)</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>these paths are relative to the parent directory selected by the user when logging in; if DicomRead="Y", path to one slice of the DICOM series is defined here</t>
   </si>
   <si>
-    <t>required for RTStruct type of image; if ROIVisibilityCode="Select" (or "Ignore") the code looks at the names in the ROI element to display or ignore</t>
-  </si>
-  <si>
     <t>names of ROI for ROIVisibilityCode="Select" or "Ignore"</t>
   </si>
   <si>
@@ -443,6 +437,12 @@
   </si>
   <si>
     <t>DefaultOrientation</t>
+  </si>
+  <si>
+    <t>required for image types = RTStruct or Segmentation; if ROIVisibilityCode="Select" (or "Ignore") the code looks at the names in the ROI element to display or ignore</t>
+  </si>
+  <si>
+    <t>(ROI name in RTStruct or Segmentation file)</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,19 +941,19 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" t="s">
-        <v>36</v>
       </c>
       <c r="G1" s="8">
         <f ca="1">TODAY()</f>
-        <v>44749</v>
+        <v>44785</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -977,13 +977,13 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -995,14 +995,14 @@
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="120" x14ac:dyDescent="0.25">
@@ -1012,14 +1012,14 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1031,16 +1031,16 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>39</v>
-      </c>
       <c r="I9" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1050,14 +1050,14 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1067,14 +1067,14 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1084,11 +1084,11 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I12" s="12"/>
     </row>
@@ -1099,14 +1099,14 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1116,14 +1116,14 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1133,14 +1133,14 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
@@ -1150,14 +1150,14 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1167,14 +1167,14 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1186,16 +1186,16 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I18" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1205,14 +1205,14 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1222,10 +1222,10 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>15</v>
@@ -1239,14 +1239,14 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1256,14 +1256,14 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I22" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1273,11 +1273,11 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I23" s="12"/>
     </row>
@@ -1288,14 +1288,14 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I24" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1305,12 +1305,12 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="165" x14ac:dyDescent="0.25">
@@ -1320,14 +1320,14 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1337,14 +1337,14 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="12" t="s">
         <v>112</v>
-      </c>
-      <c r="I27" s="12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1352,13 +1352,13 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="1"/>
       <c r="G28" s="2"/>
       <c r="H28" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I28" s="12"/>
     </row>
@@ -1367,13 +1367,13 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
       <c r="H29" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I29" s="12"/>
     </row>
@@ -1388,7 +1388,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I30" s="12"/>
     </row>
@@ -1402,13 +1402,13 @@
       <c r="E31" s="2"/>
       <c r="F31" s="1"/>
       <c r="G31" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
@@ -1420,16 +1420,16 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1443,10 +1443,10 @@
       <c r="F33" s="1"/>
       <c r="G33" s="2"/>
       <c r="H33" s="12" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1458,14 +1458,14 @@
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1475,14 +1475,14 @@
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1494,14 +1494,14 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="12" t="s">
         <v>14</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1511,10 +1511,10 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H37" s="12" t="s">
         <v>17</v>
@@ -1528,12 +1528,12 @@
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1543,12 +1543,12 @@
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1558,14 +1558,14 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I40" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>14</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,33 +1609,33 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I45" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1643,10 +1643,10 @@
         <v>0</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F48" s="18" t="s">
         <v>1</v>
@@ -1663,10 +1663,10 @@
         <v>3</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I50" s="19"/>
     </row>
@@ -1681,34 +1681,34 @@
         <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.25">
@@ -1719,23 +1719,23 @@
         <v>18</v>
       </c>
       <c r="E58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
+        <v>73</v>
+      </c>
+      <c r="H59" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="H59" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="60" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
@@ -1743,29 +1743,29 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
+        <v>62</v>
+      </c>
+      <c r="H62" s="17" t="s">
         <v>63</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="3:9" ht="30" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MOD: Added 'InitialSliceOffset' to xml Image element attributes. When the image is initially loaded, the display will be set at the mm value defined in the xml. If undefined, the image will be set to the default 'fitSliceToBackground'.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8208010B-E7A6-4059-A229-EE6AE1A47EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCC845-E7C8-43B1-B4D5-927A61732662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="140">
   <si>
     <t>Element</t>
   </si>
@@ -464,9 +464,6 @@
     <t>level value</t>
   </si>
   <si>
-    <t>Which slice was the user viewing</t>
-  </si>
-  <si>
     <t>Red, Green, Yellow, Slice4 - where this image was located on the screen</t>
   </si>
   <si>
@@ -504,6 +501,18 @@
   </si>
   <si>
     <t>required for image types = RTStruct or Segmentation; if ROIVisibilityCode="Select" (or "Ignore") the code looks at the names in the ROI subelement to display or ignore</t>
+  </si>
+  <si>
+    <t>InitialSliceOffset</t>
+  </si>
+  <si>
+    <t>Which slice was the user viewing (mm)</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>defines the slice (in mm) to display the image when initially loaded</t>
   </si>
 </sst>
 </file>
@@ -627,7 +636,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -645,9 +654,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -663,40 +669,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1013,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B63" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="I31" sqref="I30:I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1041,7 +1026,7 @@
       </c>
       <c r="G1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44791</v>
+        <v>44855</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1075,916 +1060,927 @@
       <c r="H6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="14" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="14" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12" t="s">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="14" t="s">
+      <c r="G12" s="10"/>
+      <c r="H12" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="14"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="10"/>
+      <c r="H13" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="14" t="s">
+      <c r="G14" s="10"/>
+      <c r="H14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="14" t="s">
+      <c r="G15" s="10"/>
+      <c r="H15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="14" t="s">
+      <c r="G16" s="10"/>
+      <c r="H16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="13" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="10"/>
+      <c r="H17" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="H18" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="14" t="s">
+    </row>
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11" t="s">
+      <c r="I20" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="10"/>
+      <c r="H25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="10"/>
+      <c r="H28" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="10"/>
+      <c r="H36" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+    </row>
+    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
+    </row>
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I52" s="16"/>
+    </row>
+    <row r="53" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" s="15"/>
+      <c r="H53" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I53" s="16"/>
+    </row>
+    <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G54" s="15"/>
+      <c r="H54" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I54" s="16"/>
+    </row>
+    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="16"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C56" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G26" s="11"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="144" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G27" s="11"/>
-      <c r="H27" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" s="11"/>
-      <c r="H35" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="22"/>
-      <c r="I49" s="22"/>
-    </row>
-    <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="21"/>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="22"/>
-    </row>
-    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="I51" s="22"/>
-    </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="21"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="G52" s="21"/>
-      <c r="H52" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="I52" s="22"/>
-    </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="21"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G53" s="21"/>
-      <c r="H53" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="I53" s="22"/>
-    </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="21"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="23"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="22"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C55" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H56" s="5" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F56" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F57" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F58" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F59" s="3" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F60" s="3" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F61" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F62" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F63" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H62" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D63" s="3" t="s">
+      <c r="H63" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D64" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H64" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C65" s="3" t="s">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C66" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="F66" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F66" s="3" t="s">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F67" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H66" s="5" t="s">
+      <c r="H67" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C68" s="3" t="s">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C69" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F69" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="70" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F70" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F71" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H71" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C72" s="3" t="s">
+    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C73" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D73" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H72" s="20" t="s">
+      <c r="H73" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D73" s="3" t="s">
+    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D74" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="F74" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H74" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F74" s="3" t="s">
+    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F75" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H75" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add attribute ContourVisibility to Session and Image levels to control whether contours are displayed as solids or outlines.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCC845-E7C8-43B1-B4D5-927A61732662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6BF0B8-E3B0-4400-B2EA-C3F25BC64803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="144">
   <si>
     <t>Element</t>
   </si>
@@ -513,6 +513,18 @@
   </si>
   <si>
     <t>defines the slice (in mm) to display the image when initially loaded</t>
+  </si>
+  <si>
+    <t>ContourVisibility</t>
+  </si>
+  <si>
+    <t>string 'Fill' or 'Outline' (default)</t>
+  </si>
+  <si>
+    <t>This defines how contours (label maps or segmentations) are displayed for this image. This will override the setting set at the beginning of the Session. The quiz will validate that all images for a specific destination widget (eg. Red, Green,…) have the same setting.</t>
+  </si>
+  <si>
+    <t>This defines how contours  (label maps or segmentations) are displayed for the entire quiz - as outline only or as a solid contour. This can be overridden at the Image level. (See details below.)</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="I31" sqref="I30:I31"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1026,7 +1038,7 @@
       </c>
       <c r="G1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44855</v>
+        <v>44860</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1100,397 +1112,399 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>54</v>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="10" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H10" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="13" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="13" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="13" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G19" s="10"/>
       <c r="H19" s="13" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="C20" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H20" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G21" s="11"/>
       <c r="H21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="G23" s="11"/>
       <c r="H23" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="13" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="G26" s="10"/>
-      <c r="H26" s="13"/>
+      <c r="H26" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="I26" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G27" s="10"/>
-      <c r="H27" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="H27" s="13"/>
       <c r="I27" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="13" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="13" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="10" t="s">
-        <v>108</v>
-      </c>
+      <c r="D30" s="10"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="11" t="s">
+        <v>136</v>
+      </c>
       <c r="G30" s="10"/>
       <c r="H30" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="13"/>
-    </row>
-    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>134</v>
+        <v>138</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1498,126 +1512,122 @@
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>5</v>
+        <v>108</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
       <c r="H32" s="13" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
-      <c r="G33" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="G33" s="10"/>
       <c r="H33" s="13" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E34" s="10"/>
-      <c r="F34" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10" t="s">
-        <v>8</v>
-      </c>
+      <c r="D35" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35" s="11"/>
-      <c r="G35" s="10"/>
+      <c r="G35" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="H35" s="13" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
-      <c r="C36" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="E36" s="10"/>
       <c r="F36" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G36" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="13" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="11" t="s">
-        <v>22</v>
-      </c>
+      <c r="E37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="11"/>
       <c r="G37" s="10"/>
       <c r="H37" s="13" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="C38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1627,360 +1637,396 @@
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G39" s="10"/>
       <c r="H39" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="E40" s="10"/>
       <c r="F40" s="11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G40" s="10"/>
-      <c r="H40" s="10"/>
+      <c r="H40" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="I40" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="G42" s="10"/>
-      <c r="H42" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="H42" s="10"/>
       <c r="I42" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="10"/>
+      <c r="F43" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="13" t="s">
+      <c r="F45" s="11"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I43" s="13" t="s">
+      <c r="I45" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="G44" s="15"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="G45" s="15"/>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="G46" s="15"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="15" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B50" s="15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F50" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G50" s="15"/>
-      <c r="H50" s="16"/>
-      <c r="I50" s="16"/>
-    </row>
-    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
-      <c r="C52" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="3" t="s">
-        <v>96</v>
+      <c r="C52" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="G52" s="15"/>
-      <c r="H52" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="H52" s="16"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
-      <c r="C53" s="3"/>
+      <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="F53" s="15"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="5" t="s">
-        <v>125</v>
-      </c>
+      <c r="H53" s="16"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
-      <c r="C54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="3" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="5" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="3"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="G55" s="15"/>
-      <c r="H55" s="5"/>
+      <c r="H55" s="5" t="s">
+        <v>125</v>
+      </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C56" s="3" t="s">
+    <row r="56" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="H56" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I56" s="16"/>
+    </row>
+    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="16"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H56" s="5" t="s">
+      <c r="H58" s="5" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F57" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F58" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F59" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F60" s="3" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F61" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F62" s="3" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F63" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F64" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F65" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D64" s="3" t="s">
+    <row r="66" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D66" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H66" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C66" s="3" t="s">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C68" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F67" s="3" t="s">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F69" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="H69" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C69" s="3" t="s">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F70" s="3" t="s">
+    <row r="72" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H70" s="5" t="s">
+      <c r="H72" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F71" s="3" t="s">
+    <row r="73" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F73" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H73" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C73" s="3" t="s">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C75" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H73" s="5" t="s">
+      <c r="H75" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D74" s="3" t="s">
+    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D76" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H76" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F75" s="3" t="s">
+    <row r="77" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F77" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H77" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WIP: ContourVisibility override at the Image level is working, but the coordinator needs to set things up using special rules. There is no validation being done at this point to ensure the rules are being followed to deal with the different ways that Slicer handles LabelMaps and Segmentations; eg. If a LabelMap on a 'Red' widget, all Reds must have the same visibility setting. eg. If a Segmentation for a specific Path on a 'Red' widget, all other Segmentation elements with the same Path on that page need to have the same visibility setting. (The code for LabelMap 'ShowOutline' function has to be (as is coded in this commit) turned off if processing a Segmentation node). With no validation, if the coordinator doesn't follow the rules the visibility display can be unpredictable.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6BF0B8-E3B0-4400-B2EA-C3F25BC64803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E9B79A-4FDA-416F-A84C-7EEFEAD43481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1524" yWindow="0" windowWidth="21516" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="145">
   <si>
     <t>Element</t>
   </si>
@@ -521,10 +521,13 @@
     <t>string 'Fill' or 'Outline' (default)</t>
   </si>
   <si>
-    <t>This defines how contours (label maps or segmentations) are displayed for this image. This will override the setting set at the beginning of the Session. The quiz will validate that all images for a specific destination widget (eg. Red, Green,…) have the same setting.</t>
-  </si>
-  <si>
     <t>This defines how contours  (label maps or segmentations) are displayed for the entire quiz - as outline only or as a solid contour. This can be overridden at the Image level. (See details below.)</t>
+  </si>
+  <si>
+    <t>string 'Fill' or 'Outline' (default) (To override the setting defined at the Session level)</t>
+  </si>
+  <si>
+    <t>This defines how contours (label maps or segmentations) are displayed for this image. This will override the setting defined at the beginning of the Session. NOTE: Because 3D Slicer handles images on a Layer=Segmentation differently from other Layer definitions (Foreground, Background, or Label), the quiz validation has special rules:  For images assigned to a Layer='Segmentation', all images assigned to a Segmentation layer with the same Path in this Page must have the same ContourVisibility setting. For images that are assigned to a Layer='Label'/or 'Foreground/ or 'Background', if you override the initial ContourVisibility setting here, it must match on each image with the same DefaultDestination. (eg. if you assigned visibility to 'Fill' on a 'Red' destination for a Layer='Background', all other instances of images on 'Red' must also have the same ContourVisibility='Fill' in this Page).;</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
       <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
@@ -1025,8 +1028,8 @@
     <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="67" style="5" customWidth="1"/>
-    <col min="9" max="9" width="46" style="5" customWidth="1"/>
+    <col min="8" max="8" width="43.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="52.88671875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -1038,7 +1041,7 @@
       </c>
       <c r="G1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44860</v>
+        <v>44862</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1126,7 +1129,7 @@
         <v>141</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1301,7 +1304,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10" t="s">
@@ -1356,7 +1359,7 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1490,7 +1493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="216" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1501,10 +1504,10 @@
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="9" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1539,7 +1542,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -1554,7 +1557,7 @@
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -1573,7 +1576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -1594,7 +1597,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1666,7 +1669,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -1824,7 +1827,7 @@
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="3" t="s">
@@ -1841,7 +1844,7 @@
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="3"/>
@@ -1856,7 +1859,7 @@
       </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="3"/>
@@ -1933,7 +1936,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F64" s="3" t="s">
         <v>115</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F69" s="3" t="s">
         <v>95</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F72" s="3" t="s">
         <v>72</v>
       </c>
@@ -1992,7 +1995,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F73" s="3" t="s">
         <v>59</v>
       </c>
@@ -2000,7 +2003,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
         <v>2</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D76" s="3" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Remove the override of the attribute ContourVisibility at the Image level; This will be replaced with an 'Extra Tools' option allowing the user to turn on off the Fill option for the contours.
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E9B79A-4FDA-416F-A84C-7EEFEAD43481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9028AB36-F6FB-464B-B967-3BBDCB42B9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1524" yWindow="0" windowWidth="21516" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="143">
   <si>
     <t>Element</t>
   </si>
@@ -521,13 +521,7 @@
     <t>string 'Fill' or 'Outline' (default)</t>
   </si>
   <si>
-    <t>This defines how contours  (label maps or segmentations) are displayed for the entire quiz - as outline only or as a solid contour. This can be overridden at the Image level. (See details below.)</t>
-  </si>
-  <si>
-    <t>string 'Fill' or 'Outline' (default) (To override the setting defined at the Session level)</t>
-  </si>
-  <si>
-    <t>This defines how contours (label maps or segmentations) are displayed for this image. This will override the setting defined at the beginning of the Session. NOTE: Because 3D Slicer handles images on a Layer=Segmentation differently from other Layer definitions (Foreground, Background, or Label), the quiz validation has special rules:  For images assigned to a Layer='Segmentation', all images assigned to a Segmentation layer with the same Path in this Page must have the same ContourVisibility setting. For images that are assigned to a Layer='Label'/or 'Foreground/ or 'Background', if you override the initial ContourVisibility setting here, it must match on each image with the same DefaultDestination. (eg. if you assigned visibility to 'Fill' on a 'Red' destination for a Layer='Background', all other instances of images on 'Red' must also have the same ContourVisibility='Fill' in this Page).;</t>
+    <t>This defines how contours  (label maps or segmentations) are displayed for the entire quiz - as outline only or as a solid contour.</t>
   </si>
 </sst>
 </file>
@@ -1013,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C29" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1115,7 +1109,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1493,137 +1487,137 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="216" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I31" s="9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
       <c r="H32" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
       <c r="G33" s="10"/>
       <c r="H33" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="10"/>
+      <c r="G34" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="H34" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I34" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" s="10"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="14" t="s">
+      <c r="F35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="12" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="10"/>
       <c r="H36" s="13" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
+      <c r="C37" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D37" s="10"/>
-      <c r="E37" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" s="11"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="G37" s="10"/>
       <c r="H37" s="13" t="s">
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="11" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="13" t="s">
@@ -1637,7 +1631,9 @@
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="10"/>
+      <c r="D39" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="E39" s="10"/>
       <c r="F39" s="11" t="s">
         <v>22</v>
@@ -1647,53 +1643,49 @@
         <v>14</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G40" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H40" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H41" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -1701,54 +1693,47 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="11" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
+      <c r="H43" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="I43" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="11" t="s">
-        <v>101</v>
-      </c>
+      <c r="E44" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="11"/>
       <c r="G44" s="10"/>
-      <c r="H44" s="11" t="s">
-        <v>103</v>
+      <c r="H44" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>102</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="10"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="G45" s="15"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
@@ -1758,278 +1743,270 @@
       <c r="E46" s="15"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="G47" s="15"/>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="15" t="s">
+      <c r="B49" s="15" t="s">
         <v>76</v>
       </c>
+    </row>
+    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E51" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="16"/>
     </row>
     <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
-      <c r="C52" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D52" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>1</v>
-      </c>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
+      <c r="C53" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
+      <c r="F53" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="G53" s="15"/>
-      <c r="H53" s="16"/>
+      <c r="H53" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
-      <c r="C54" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C54" s="3"/>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="3" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="3"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="3" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="3"/>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
-      <c r="F56" s="3" t="s">
-        <v>58</v>
-      </c>
+      <c r="F56" s="3"/>
       <c r="G56" s="15"/>
-      <c r="H56" s="5" t="s">
-        <v>126</v>
-      </c>
+      <c r="H56" s="5"/>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="16"/>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>44</v>
+      <c r="F58" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F59" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F60" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F61" s="3" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F62" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F63" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F64" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D65" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C67" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F68" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C70" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F71" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H62" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F63" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F64" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="F65" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H65" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D66" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H66" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C68" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="69" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F69" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H69" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C71" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>60</v>
+      <c r="H71" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F72" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="73" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="F73" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C74" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D75" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H73" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C75" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="H75" s="5" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D76" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="F76" s="3" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="77" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F77" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H77" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added  Query to user to email results upon completion of the quiz, or when re-opening the quiz for review FIX: setting the bEmailResults variable for the Session
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F910791-B05A-4073-922B-B6732F871B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1524" yWindow="0" windowWidth="21516" windowHeight="10704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1530" yWindow="0" windowWidth="21510" windowHeight="10710"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="147">
   <si>
     <t>Element</t>
   </si>
@@ -488,9 +487,6 @@
     <t>ID string used for matching if an Image on a subsequent Page needs this Label Map displayed; (If more than one image element is set up for this image path - differing orientations, this attribute only needs to be set up on one instance)</t>
   </si>
   <si>
-    <t>to rotate the image to the plane of acquisition</t>
-  </si>
-  <si>
     <t>If "Y", the user must create a segment (case: a tumor is present in the scan and the user must find it); For the resulting label map file: 1) an empty label map is not accepted; 2) if a label map file is redisplayed from a previous page (using DisplayLabelMapID), modification of the label map is required; NOTE: if this attribute appears on an image that is displayed in more than one viewing window, it must be repeated for each; This attribute is not applicable for images assigned to a Layer = Segmentation or Label ;</t>
   </si>
   <si>
@@ -525,12 +521,24 @@
   </si>
   <si>
     <t>Note: for time series 'VolumeSequence' type images, if being read in using DicomRead="Y", all dicom files must be located in the same folder (no subfolders separating the time sequences).</t>
+  </si>
+  <si>
+    <t>EmailResultsTo</t>
+  </si>
+  <si>
+    <t>string holding email address to receive results</t>
+  </si>
+  <si>
+    <t>see documentation on how to configure the smtp server</t>
+  </si>
+  <si>
+    <t>to rotate the view to the plane of acquisition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1009,27 +1017,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.5546875" style="5" customWidth="1"/>
-    <col min="9" max="9" width="52.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43.5703125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="52.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1038,16 +1046,16 @@
       </c>
       <c r="G1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>44909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1084,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1103,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1112,517 +1120,517 @@
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I9" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="10"/>
+        <v>37</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H11" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="13" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="11" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="11" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="13" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="11" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="11" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="13" t="s">
         <v>27</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="13" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="11" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="13" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="G20" s="10"/>
       <c r="H20" s="13" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="C21" s="10" t="s">
+        <v>4</v>
+      </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="11"/>
+        <v>37</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H21" s="13" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G22" s="11"/>
       <c r="H22" s="13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="11"/>
+        <v>23</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H23" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="G24" s="11"/>
       <c r="H24" s="13" t="s">
         <v>14</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="11" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="13" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G26" s="10"/>
       <c r="H26" s="13" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="11" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
+      <c r="H27" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="I27" s="13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="11" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G28" s="10"/>
-      <c r="H28" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="H28" s="13"/>
       <c r="I28" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="11" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="13" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="11" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="13" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="10" t="s">
-        <v>108</v>
-      </c>
+      <c r="D31" s="10"/>
       <c r="E31" s="10"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="11" t="s">
+        <v>135</v>
+      </c>
       <c r="G31" s="10"/>
       <c r="H31" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I31" s="13"/>
-    </row>
-    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="11"/>
       <c r="G32" s="10"/>
       <c r="H32" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="E33" s="10"/>
       <c r="F33" s="11"/>
       <c r="G33" s="10"/>
       <c r="H33" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="G34" s="10"/>
       <c r="H34" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="10"/>
-      <c r="F35" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="12" t="s">
+      <c r="F35" s="11"/>
+      <c r="G35" s="14" t="s">
         <v>29</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="10"/>
+      <c r="F36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="H36" s="13" t="s">
-        <v>110</v>
+        <v>26</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
-      <c r="C37" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="C37" s="10"/>
       <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="11" t="s">
-        <v>37</v>
-      </c>
+      <c r="E37" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="11"/>
       <c r="G37" s="10"/>
       <c r="H37" s="13" t="s">
-        <v>14</v>
+        <v>110</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
+      <c r="C38" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="11" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="13" t="s">
@@ -1632,13 +1640,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="10" t="s">
-        <v>16</v>
-      </c>
+      <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="11" t="s">
         <v>22</v>
@@ -1648,49 +1654,53 @@
         <v>14</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="E40" s="10"/>
       <c r="F40" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G40" s="10"/>
       <c r="H40" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
@@ -1698,49 +1708,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
       <c r="F43" s="11" t="s">
-        <v>101</v>
+        <v>31</v>
       </c>
       <c r="G43" s="10"/>
-      <c r="H43" s="11" t="s">
-        <v>103</v>
-      </c>
+      <c r="H43" s="10"/>
       <c r="I43" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="10"/>
+      <c r="F44" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="10"/>
-      <c r="H44" s="13" t="s">
+      <c r="F45" s="11"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I44" s="13" t="s">
+      <c r="I45" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="G45" s="15"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -1748,270 +1765,278 @@
       <c r="E46" s="15"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="15" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G51" s="15"/>
-      <c r="H51" s="16"/>
-      <c r="I51" s="16"/>
-    </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
+      <c r="C52" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>1</v>
+      </c>
       <c r="G52" s="15"/>
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
-      <c r="C53" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="C53" s="15"/>
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
-      <c r="F53" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="F53" s="15"/>
       <c r="G53" s="15"/>
-      <c r="H53" s="5" t="s">
-        <v>97</v>
-      </c>
+      <c r="H53" s="16"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
-      <c r="C54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="3" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="5" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="3"/>
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="3" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="3"/>
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="G56" s="15"/>
-      <c r="H56" s="5"/>
+      <c r="H56" s="5" t="s">
+        <v>126</v>
+      </c>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C57" s="3" t="s">
+    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="16"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D58" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="H58" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F58" s="3" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F59" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H58" s="5" t="s">
+      <c r="H59" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F59" s="3" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F60" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="H60" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F60" s="3" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F61" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="H60" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F61" s="3" t="s">
+      <c r="H61" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F62" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H62" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F62" s="3" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F63" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="H63" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F63" s="3" t="s">
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="F64" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H64" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F64" s="3" t="s">
+    <row r="65" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F65" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D65" s="3" t="s">
+    <row r="66" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="H66" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C67" s="3" t="s">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F68" s="3" t="s">
+    <row r="69" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F69" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="H69" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C70" s="3" t="s">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E71" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="F71" s="3" t="s">
+    <row r="72" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="F72" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H71" s="5" t="s">
+      <c r="H72" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="F72" s="3" t="s">
+    <row r="73" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="F73" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="H73" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C74" s="3" t="s">
+    <row r="75" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H74" s="5" t="s">
+      <c r="H75" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D75" s="3" t="s">
+    <row r="76" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="D76" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H75" s="5" t="s">
+      <c r="H76" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="F76" s="3" t="s">
+    <row r="77" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F77" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="H76" s="5" t="s">
+      <c r="H77" s="5" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Release Time Line document - includes ties to master and dev branches which are pushed to public repo BainesImageQuizzer
</commit_message>
<xml_diff>
--- a/Documentation/XML ElementsAndAttributes.xlsx
+++ b/Documentation/XML ElementsAndAttributes.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\cjohnson\Work\Projects\SlicerEclipseProjects\ImageQuizzerProject\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alibi\Documents\Work-Baines\Projects\ImageQuizzer\ImageQuizzerProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2936C0B9-4183-48DD-97A4-8EC762C291B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="0" windowWidth="21510" windowHeight="10710"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="148">
   <si>
     <t>Element</t>
   </si>
@@ -534,11 +537,14 @@
   <si>
     <t>TwoOverTwo, FourUp, OneUpRedSlice, SideBySideRedYellow (default=FourUp)</t>
   </si>
+  <si>
+    <t>v2.2.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -601,7 +607,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -652,11 +658,190 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -703,6 +888,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1017,27 +1247,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.5703125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="52.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="43.5546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="52.88671875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -1046,16 +1276,16 @@
       </c>
       <c r="G1" s="4">
         <f ca="1">TODAY()</f>
-        <v>44985</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1314,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1333,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1120,7 +1350,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1137,7 +1367,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1154,7 +1384,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="s">
         <v>3</v>
@@ -1175,7 +1405,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1192,7 +1422,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1209,7 +1439,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1224,7 +1454,7 @@
       </c>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1241,7 +1471,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1258,7 +1488,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1275,7 +1505,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1292,7 +1522,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1309,7 +1539,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="165" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1326,7 +1556,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
@@ -1347,7 +1577,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -1364,7 +1594,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1383,7 +1613,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -1400,7 +1630,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -1417,7 +1647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1434,7 +1664,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1451,7 +1681,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -1466,7 +1696,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1483,7 +1713,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1500,7 +1730,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1517,7 +1747,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1532,7 +1762,7 @@
       </c>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1549,7 +1779,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -1564,7 +1794,7 @@
       </c>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -1583,7 +1813,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -1604,7 +1834,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -1621,7 +1851,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10" t="s">
@@ -1640,7 +1870,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -1657,7 +1887,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -1676,7 +1906,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -1693,7 +1923,7 @@
       </c>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1708,7 +1938,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -1723,7 +1953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1740,7 +1970,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -1757,7 +1987,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -1765,7 +1995,7 @@
       <c r="E46" s="15"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -1773,7 +2003,7 @@
       <c r="E47" s="15"/>
       <c r="G47" s="15"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
         <v>76</v>
       </c>
@@ -1799,12 +2029,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B50" s="15" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15" t="s">
@@ -1823,7 +2053,7 @@
       <c r="H52" s="16"/>
       <c r="I52" s="16"/>
     </row>
-    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -1834,7 +2064,7 @@
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
     </row>
-    <row r="54" spans="1:9" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="3" t="s">
@@ -1851,7 +2081,7 @@
       </c>
       <c r="I54" s="16"/>
     </row>
-    <row r="55" spans="1:9" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="1" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="3"/>
@@ -1866,7 +2096,7 @@
       </c>
       <c r="I55" s="16"/>
     </row>
-    <row r="56" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
       <c r="B56" s="15"/>
       <c r="C56" s="3"/>
@@ -1881,7 +2111,7 @@
       </c>
       <c r="I56" s="16"/>
     </row>
-    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="3"/>
@@ -1892,7 +2122,7 @@
       <c r="H57" s="5"/>
       <c r="I57" s="16"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C58" s="3" t="s">
         <v>4</v>
       </c>
@@ -1903,7 +2133,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F59" s="3" t="s">
         <v>111</v>
       </c>
@@ -1911,7 +2141,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F60" s="3" t="s">
         <v>112</v>
       </c>
@@ -1919,7 +2149,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F61" s="3" t="s">
         <v>113</v>
       </c>
@@ -1927,7 +2157,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F62" s="3" t="s">
         <v>71</v>
       </c>
@@ -1935,7 +2165,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F63" s="3" t="s">
         <v>116</v>
       </c>
@@ -1943,7 +2173,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F64" s="3" t="s">
         <v>114</v>
       </c>
@@ -1951,7 +2181,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="65" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
       <c r="F65" s="3" t="s">
         <v>115</v>
       </c>
@@ -1959,7 +2189,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D66" s="3" t="s">
         <v>45</v>
       </c>
@@ -1967,7 +2197,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C68" s="3" t="s">
         <v>46</v>
       </c>
@@ -1975,7 +2205,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F69" s="3" t="s">
         <v>94</v>
       </c>
@@ -1983,7 +2213,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C71" s="3" t="s">
         <v>16</v>
       </c>
@@ -1994,7 +2224,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F72" s="3" t="s">
         <v>71</v>
       </c>
@@ -2002,7 +2232,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="3:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F73" s="3" t="s">
         <v>58</v>
       </c>
@@ -2010,7 +2240,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C75" s="3" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +2251,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D76" s="3" t="s">
         <v>46</v>
       </c>
@@ -2032,7 +2262,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F77" s="3" t="s">
         <v>80</v>
       </c>
@@ -2044,4 +2274,481 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9E65CE-BF8F-452F-A546-AF1ACECB9BEE}">
+  <dimension ref="A1:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="E1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="4">
+        <f ca="1">TODAY()</f>
+        <v>45035</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="23"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="23"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="23"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="23"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="25" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="23"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="23"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="23"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="23"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="23"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="23"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="26"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="23"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="23"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="23"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="23"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="23"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="23"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>